<commit_message>
Updating data from sites and FishDB for the ETP. Species richness graphs and MaxN per hour graphs for fish community, predators and sharks. PERMANOVA and PCO analyses for fish community, predators and sharks.
</commit_message>
<xml_diff>
--- a/Data/Malpelo_2015_Length.xlsx
+++ b/Data/Malpelo_2015_Length.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Desktop\BRUVS ETP Data\Excel sheets for analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Desktop\BRUVS_ETP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95DFB112-3385-4B37-9777-3AEBB7B664DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB127DD2-77A6-4B1B-98B7-BBABD56CCEEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9FC7783A-2F0D-41C0-AE61-71967F9D479D}"/>
   </bookViews>
@@ -854,9 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AFCF73E-12F2-479E-889A-28A853974BDD}">
   <dimension ref="A1:AI256"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>